<commit_message>
vertical Lines + Measures + Measure Selection
</commit_message>
<xml_diff>
--- a/Tableau/Input/measures.xlsx
+++ b/Tableau/Input/measures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIDA\CertProjCovid19\Tableau\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB752D9B-6A90-4582-9E3D-FA1656C7551D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE2986DE-1CA7-48D5-B58E-82E8CF4B3B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E70B0121-EF8F-4CE9-8441-FAD9795C48F3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Germany</t>
+  </si>
+  <si>
+    <t>just a day</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
@@ -413,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF75D93-EF29-4C28-8809-CBA2BD8E3E74}">
   <dimension ref="A1:C367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,82 +1391,88 @@
         <v>44021</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44022</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44023</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44024</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44025</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44026</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44027</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44028</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44030</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44032</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44033</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44034</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44035</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44037</v>
       </c>

</xml_diff>